<commit_message>
report & stats update
</commit_message>
<xml_diff>
--- a/reports/templates/daily-store.xlsx
+++ b/reports/templates/daily-store.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uicestone/Sites/minimars-server/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D728A19-1006-7E42-A4F7-6432917E2037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D7EB23-E5C7-744C-8E1E-46B45E3C5311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1000" windowWidth="26840" windowHeight="16440" xr2:uid="{4F58C902-78D5-2145-A3CE-3267BB3BABFE}"/>
+    <workbookView xWindow="-6280" yWindow="5800" windowWidth="26840" windowHeight="16440" xr2:uid="{4F58C902-78D5-2145-A3CE-3267BB3BABFE}"/>
   </bookViews>
   <sheets>
     <sheet name="门店日报" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>到店组数</t>
   </si>
@@ -51,30 +51,9 @@
     <t>门票收入</t>
   </si>
   <si>
-    <t>活动收入</t>
-  </si>
-  <si>
-    <t>餐饮收入</t>
-  </si>
-  <si>
-    <t>当日店内点单餐饮收入</t>
-  </si>
-  <si>
-    <t>派对零点餐饮收入</t>
-  </si>
-  <si>
     <t>派对收入</t>
   </si>
   <si>
-    <t>派对套系收入</t>
-  </si>
-  <si>
-    <t>派对自助套餐餐饮收入</t>
-  </si>
-  <si>
-    <t>派对其他收入</t>
-  </si>
-  <si>
     <t>外拓收入（权责）</t>
   </si>
   <si>
@@ -152,10 +131,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>余额消费按实充额折算</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>吧台销售储值卡数目前合并计入在10行中</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -200,12 +175,6 @@
     <t>${playAmount}</t>
   </si>
   <si>
-    <t>${eventAmount}</t>
-  </si>
-  <si>
-    <t>${foodAmount}</t>
-  </si>
-  <si>
     <t>${partyAmount}</t>
   </si>
   <si>
@@ -255,6 +224,18 @@
   </si>
   <si>
     <t>${couponPlayAmount}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 派对套系收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 派对自助套餐餐饮收入</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>- 派对其他收入</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8EA64C-3023-A04F-8D77-D73A58D0B3BC}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -683,7 +664,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21">
       <c r="A1" s="8" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -693,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -701,49 +682,49 @@
         <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="e">
         <f t="shared" ref="B8" si="0">B9+B10+B11</f>
@@ -752,50 +733,50 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -812,10 +793,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -823,10 +804,10 @@
         <v>4</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -834,193 +815,162 @@
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="2" t="e">
-        <f>B22+B23+B24+B27+B31+B32</f>
+        <v>11</v>
+      </c>
+      <c r="B21" s="6" t="e">
+        <f>B23/B3</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>13</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>39</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4"/>
+        <v>15</v>
+      </c>
+      <c r="B25" s="7" t="e">
+        <f>B24/B23</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="4"/>
+        <v>16</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>13</v>
-      </c>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" s="4"/>
+        <v>18</v>
+      </c>
+      <c r="B28" s="7" t="e">
+        <f>B26/B23</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="B30" s="7" t="e">
+        <f>B31/B3</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="4"/>
+        <v>20</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="6" t="e">
-        <f>B36/B3</f>
-        <v>#VALUE!</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>19</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="B37" s="2" t="e">
+        <f>B38+#REF!+#REF!+B39+B43+B44</f>
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="7" t="e">
-        <f>B37/B36</f>
-        <v>#VALUE!</v>
+        <v>7</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>23</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" t="s">
-        <v>40</v>
+        <v>8</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>24</v>
+      <c r="A40" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B40" s="4"/>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="7" t="e">
-        <f>B39/B36</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="A41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="4"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="4"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="4"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="7" t="e">
-        <f>B45/B3</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
-        <v>27</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>30</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
food sets count in dashboard and report
</commit_message>
<xml_diff>
--- a/reports/templates/daily-store.xlsx
+++ b/reports/templates/daily-store.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uicestone/Sites/minimars-server/reports/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093F6369-3D09-6E4A-9572-8796238E630B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BCB364-A2BF-7045-9239-4B773045096A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="12880" windowHeight="17500" xr2:uid="{4F58C902-78D5-2145-A3CE-3267BB3BABFE}"/>
   </bookViews>
@@ -19,6 +19,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -244,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>到店组数</t>
   </si>
@@ -480,6 +487,10 @@
   </si>
   <si>
     <t>会员续卡率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>${foodSetsCount}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -923,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8EA64C-3023-A04F-8D77-D73A58D0B3BC}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1156,7 +1167,9 @@
       <c r="A28" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="5"/>
+      <c r="B28" s="5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">

</xml_diff>